<commit_message>
fix excel input of variables + make diagramm (tablitsa)0.1.9.0
</commit_message>
<xml_diff>
--- a/Коэффициенты_f.XLSX
+++ b/Коэффициенты_f.XLSX
@@ -14,7 +14,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="56" uniqueCount="55">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="58" uniqueCount="57">
   <si>
     <t>ВЛ8</t>
   </si>
@@ -179,6 +179,12 @@
   </si>
   <si>
     <t>8-осный</t>
+  </si>
+  <si>
+    <t>ТЭ10</t>
+  </si>
+  <si>
+    <t>2ТЭ10</t>
   </si>
 </sst>
 </file>
@@ -188,13 +194,20 @@
   <numFmts count="1">
     <numFmt numFmtId="164" formatCode="0.0000"/>
   </numFmts>
-  <fonts count="1" x14ac:knownFonts="1">
+  <fonts count="2" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="10"/>
+      <color rgb="FF6A8759"/>
+      <name val="Arial Unicode MS"/>
+      <family val="2"/>
+      <charset val="204"/>
     </font>
   </fonts>
   <fills count="2">
@@ -217,11 +230,14 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="4">
+  <cellXfs count="5">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" quotePrefix="1" applyNumberFormat="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Обычный" xfId="0" builtinId="0"/>
@@ -526,10 +542,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:Q52"/>
+  <dimension ref="A1:Q54"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A37" workbookViewId="0">
-      <selection activeCell="M56" sqref="M56"/>
+      <selection activeCell="A54" sqref="A54"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -658,43 +674,43 @@
         <v>1.27</v>
       </c>
       <c r="D3" s="1">
-        <f t="shared" ref="D3:D49" si="0">(E3+C3)/2</f>
+        <f t="shared" ref="D3:D47" si="0">(E3+C3)/2</f>
         <v>1.2725</v>
       </c>
       <c r="E3">
-        <f t="shared" ref="E3:E49" si="1">(C3+G3)/2</f>
+        <f t="shared" ref="E3:E47" si="1">(C3+G3)/2</f>
         <v>1.2749999999999999</v>
       </c>
       <c r="F3">
-        <f t="shared" ref="F3:F49" si="2">(E3+G3)/2</f>
+        <f t="shared" ref="F3:F47" si="2">(E3+G3)/2</f>
         <v>1.2774999999999999</v>
       </c>
       <c r="G3">
         <v>1.28</v>
       </c>
       <c r="H3">
-        <f t="shared" ref="H3:H49" si="3">(G3+I3)/2</f>
+        <f t="shared" ref="H3:H47" si="3">(G3+I3)/2</f>
         <v>1.29</v>
       </c>
       <c r="I3">
         <v>1.3</v>
       </c>
       <c r="J3">
-        <f t="shared" ref="J3:J49" si="4">(K3+I3)/2</f>
+        <f t="shared" ref="J3:J47" si="4">(K3+I3)/2</f>
         <v>1.3149999999999999</v>
       </c>
       <c r="K3">
         <v>1.33</v>
       </c>
       <c r="L3">
-        <f t="shared" ref="L3:L49" si="5">(K3+M3)/2</f>
+        <f t="shared" ref="L3:L47" si="5">(K3+M3)/2</f>
         <v>1.35</v>
       </c>
       <c r="M3">
         <v>1.37</v>
       </c>
       <c r="N3">
-        <f t="shared" ref="N3:N49" si="6">(O3+M3)/2</f>
+        <f t="shared" ref="N3:N47" si="6">(O3+M3)/2</f>
         <v>1.3900000000000001</v>
       </c>
       <c r="O3">
@@ -3645,6 +3661,126 @@
       </c>
       <c r="Q52">
         <v>1.62</v>
+      </c>
+    </row>
+    <row r="53" spans="1:17" x14ac:dyDescent="0.3">
+      <c r="A53" t="s">
+        <v>55</v>
+      </c>
+      <c r="B53">
+        <v>1.1000000000000001</v>
+      </c>
+      <c r="C53">
+        <v>1.1599999999999999</v>
+      </c>
+      <c r="D53" s="1">
+        <f t="shared" ref="D53:D54" si="14">(E53+C53)/2</f>
+        <v>1.19</v>
+      </c>
+      <c r="E53">
+        <f t="shared" ref="E53:E54" si="15">(C53+G53)/2</f>
+        <v>1.22</v>
+      </c>
+      <c r="F53">
+        <f t="shared" ref="F53:F54" si="16">(E53+G53)/2</f>
+        <v>1.25</v>
+      </c>
+      <c r="G53">
+        <v>1.28</v>
+      </c>
+      <c r="H53">
+        <f t="shared" ref="H53:H54" si="17">(G53+I53)/2</f>
+        <v>1.31</v>
+      </c>
+      <c r="I53">
+        <v>1.34</v>
+      </c>
+      <c r="J53">
+        <f t="shared" ref="J53:J54" si="18">(K53+I53)/2</f>
+        <v>1.385</v>
+      </c>
+      <c r="K53">
+        <v>1.43</v>
+      </c>
+      <c r="L53">
+        <f t="shared" ref="L53:L54" si="19">(K53+M53)/2</f>
+        <v>1.48</v>
+      </c>
+      <c r="M53">
+        <v>1.53</v>
+      </c>
+      <c r="N53">
+        <f t="shared" ref="N53:N54" si="20">(O53+M53)/2</f>
+        <v>1.585</v>
+      </c>
+      <c r="O53">
+        <v>1.64</v>
+      </c>
+      <c r="P53">
+        <v>1.7</v>
+      </c>
+      <c r="Q53">
+        <v>1.75</v>
+      </c>
+    </row>
+    <row r="54" spans="1:17" ht="15" x14ac:dyDescent="0.3">
+      <c r="A54" s="4" t="s">
+        <v>56</v>
+      </c>
+      <c r="B54">
+        <v>1.1299999999999999</v>
+      </c>
+      <c r="C54">
+        <v>1.2</v>
+      </c>
+      <c r="D54" s="1">
+        <f t="shared" si="14"/>
+        <v>1.2124999999999999</v>
+      </c>
+      <c r="E54">
+        <f t="shared" si="15"/>
+        <v>1.2250000000000001</v>
+      </c>
+      <c r="F54">
+        <f t="shared" si="16"/>
+        <v>1.2375</v>
+      </c>
+      <c r="G54">
+        <v>1.25</v>
+      </c>
+      <c r="H54">
+        <f t="shared" si="17"/>
+        <v>1.2749999999999999</v>
+      </c>
+      <c r="I54">
+        <v>1.3</v>
+      </c>
+      <c r="J54">
+        <f t="shared" si="18"/>
+        <v>1.3250000000000002</v>
+      </c>
+      <c r="K54">
+        <v>1.35</v>
+      </c>
+      <c r="L54">
+        <f t="shared" si="19"/>
+        <v>1.375</v>
+      </c>
+      <c r="M54">
+        <v>1.4</v>
+      </c>
+      <c r="N54">
+        <f t="shared" si="20"/>
+        <v>1.45</v>
+      </c>
+      <c r="O54">
+        <v>1.5</v>
+      </c>
+      <c r="P54">
+        <v>1.6</v>
+      </c>
+      <c r="Q54">
+        <v>1.7</v>
       </c>
     </row>
   </sheetData>

</xml_diff>